<commit_message>
Add a new todo list
</commit_message>
<xml_diff>
--- a/TODO SimPancake 3000.xlsx
+++ b/TODO SimPancake 3000.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ashley Sands\Amstrike Games\SimPancake3000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5296B1C-3203-4F67-9B7A-C308E85195EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788857D9-A528-4CF1-BC23-319337E26870}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6732AF01-4E77-4178-A282-B4B033BA40EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6732AF01-4E77-4178-A282-B4B033BA40EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="87">
   <si>
     <t>Project Sheet - Summary</t>
   </si>
@@ -289,6 +289,24 @@
   </si>
   <si>
     <t>Replace Jug Gyro</t>
+  </si>
+  <si>
+    <t>Make batter trails look better</t>
+  </si>
+  <si>
+    <t>ie. Mix the trails color up a lil</t>
+  </si>
+  <si>
+    <t>Improve batter spread</t>
+  </si>
+  <si>
+    <t>Add dynamic pancake spreed</t>
+  </si>
+  <si>
+    <t>Make pancakes cook</t>
+  </si>
+  <si>
+    <t>Add AI</t>
   </si>
 </sst>
 </file>
@@ -1487,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30403D6D-C9A3-4C64-B0D0-8C03B84E3440}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1582,7 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">_xlfn.DAYS(E4,NOW())</f>
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>6</v>
@@ -1581,7 +1599,7 @@
       </c>
       <c r="C6" s="12">
         <f ca="1">1-IF(E5&lt;&gt;0,(C5/E5),0)</f>
-        <v>0.29032258064516125</v>
+        <v>0.64516129032258063</v>
       </c>
       <c r="D6" s="89" t="s">
         <v>8</v>
@@ -1606,7 +1624,7 @@
       </c>
       <c r="C9" s="14">
         <f>C17+C18+C19+G17+G18+G19</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>11</v>
@@ -1620,14 +1638,14 @@
       </c>
       <c r="G9" s="14">
         <f>C9+E9</f>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="17">
         <f>C15+G15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1636,14 +1654,14 @@
       </c>
       <c r="C10" s="18">
         <f>C9/G9</f>
-        <v>0.41666666666666669</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="19">
         <f>E9/G9</f>
-        <v>0.58333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>14</v>
@@ -1657,7 +1675,7 @@
       </c>
       <c r="I10" s="21">
         <f>I9/G9</f>
-        <v>0</v>
+        <v>3.5714285714285712E-2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1665,7 +1683,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="18">
-        <v>0.41666666666666702</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1697,11 +1715,11 @@
       </c>
       <c r="C14" s="24">
         <f>COUNTIF(Main[Status], "-")</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="25">
         <f>C14/C20</f>
-        <v>0.625</v>
+        <v>0.45</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="23" t="s">
@@ -1713,7 +1731,7 @@
       </c>
       <c r="H14" s="25">
         <f>G14/G20</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1722,11 +1740,11 @@
       </c>
       <c r="C15" s="24">
         <f>COUNTIF(Main[Status], "wip")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="25">
         <f>C15/C20</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="23" t="s">
@@ -1772,11 +1790,11 @@
       </c>
       <c r="C17" s="24">
         <f>COUNTIF(Main[Status], "c")</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D17" s="25">
         <f>C17/C20</f>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="23" t="s">
@@ -1788,7 +1806,7 @@
       </c>
       <c r="H17" s="25">
         <f>G17/G20</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1847,7 +1865,7 @@
       </c>
       <c r="C20" s="28">
         <f>COUNTA(Main[Status])</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D20" s="29">
         <f>SUM(D14:D19)</f>
@@ -1859,11 +1877,11 @@
       </c>
       <c r="G20" s="28">
         <f>COUNTA(Main[Status])</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H20" s="29">
         <f>SUM(H14:H19)</f>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1872,14 +1890,14 @@
       </c>
       <c r="C21" s="30">
         <f>D14+D15+D16</f>
-        <v>0.625</v>
+        <v>0.5</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>24</v>
       </c>
       <c r="G21" s="30">
         <f>H14+H15+H16</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="S21" s="67"/>
     </row>
@@ -1889,14 +1907,14 @@
       </c>
       <c r="C22" s="32">
         <f>D17+D18+D19</f>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F22" s="31" t="s">
         <v>25</v>
       </c>
       <c r="G22" s="32">
         <f>H17+H18+H19</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2037,11 +2055,11 @@
       </c>
       <c r="N28" s="50">
         <f>D28/G9</f>
-        <v>0.29166666666666669</v>
+        <v>0.25</v>
       </c>
       <c r="O28" s="65">
         <f>N28</f>
-        <v>0.29166666666666669</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -2052,20 +2070,17 @@
         <v>43612</v>
       </c>
       <c r="C29" s="41">
-        <f>G9</f>
         <v>24</v>
       </c>
       <c r="D29" s="42">
-        <f>C9</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E29" s="42">
-        <f t="shared" ref="E29:E32" si="0">C29-D29</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F29" s="43">
-        <f t="shared" ref="F29:F32" si="1">D29/C29</f>
-        <v>0.41666666666666669</v>
+        <f t="shared" ref="F29:F32" si="0">D29/C29</f>
+        <v>0.45833333333333331</v>
       </c>
       <c r="G29" s="44">
         <f>C29-C28</f>
@@ -2077,31 +2092,31 @@
       </c>
       <c r="I29" s="44">
         <f>D29-D28</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J29" s="46">
         <f>(I29-I28)/I28</f>
-        <v>-0.5714285714285714</v>
+        <v>-0.42857142857142855</v>
       </c>
       <c r="K29" s="47">
-        <f t="shared" ref="K29" si="2">I29/G29</f>
-        <v>0.75</v>
+        <f t="shared" ref="K29" si="1">I29/G29</f>
+        <v>1</v>
       </c>
       <c r="L29" s="48">
         <f ca="1">IF(NOW()&lt;B29, G29/_xlfn.DAYS(NOW(),B28), G29/_xlfn.DAYS(B29,B28))</f>
-        <v>1</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="M29" s="49">
         <f ca="1">IF(NOW()&lt;B29, I29/_xlfn.DAYS(NOW(),B28), I29/_xlfn.DAYS(B29,B28))</f>
-        <v>0.75</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="N29" s="50">
         <f>D29/G9</f>
-        <v>0.41666666666666669</v>
+        <v>0.39285714285714285</v>
       </c>
       <c r="O29" s="65">
-        <f>N29</f>
-        <v>0.41666666666666669</v>
+        <f>N29-O28</f>
+        <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -2112,54 +2127,54 @@
         <v>43619</v>
       </c>
       <c r="C30" s="41">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D30" s="42">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E30" s="42">
+        <f t="shared" ref="E30:E32" si="2">C30-D30</f>
+        <v>16</v>
+      </c>
+      <c r="F30" s="43">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="43" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="G30" s="44">
         <f>C30-C29</f>
-        <v>-24</v>
+        <v>4</v>
       </c>
       <c r="H30" s="45">
         <f t="shared" ref="H30:H32" si="3">(G30-G29)/G29</f>
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="I30" s="44">
         <f t="shared" ref="I30:I31" si="4">D30-0</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J30" s="46">
         <f t="shared" ref="J30:J32" si="5">(I30-I29)/I29</f>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="K30" s="47">
         <f t="shared" ref="K30:K31" si="6">I30/G30</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L30" s="48">
         <f ca="1">IF(NOW()&lt;B30, G30/_xlfn.DAYS(NOW(),B29), G30/_xlfn.DAYS(B30,B29))</f>
-        <v>8</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="M30" s="49">
         <f t="shared" ref="M30:M31" ca="1" si="7">IF(NOW()&lt;B30, I30/_xlfn.DAYS(NOW(),B29), I30/_xlfn.DAYS(B30,B29))</f>
-        <v>0</v>
+        <v>1.7142857142857142</v>
       </c>
       <c r="N30" s="50">
         <f>D30/G9</f>
-        <v>0</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="O30" s="65">
-        <f t="shared" ref="O30:O32" si="8">N30</f>
-        <v>0</v>
+        <f t="shared" ref="O30:O32" si="8">N30-O29</f>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -2176,36 +2191,36 @@
         <v>0</v>
       </c>
       <c r="E31" s="42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="43" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="43" t="e">
-        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G31" s="44">
-        <f t="shared" ref="G30:G32" si="9">C31-C30</f>
-        <v>0</v>
+        <f t="shared" ref="G31:G32" si="9">C31-C30</f>
+        <v>-28</v>
       </c>
       <c r="H31" s="45">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>-8</v>
       </c>
       <c r="I31" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J31" s="46" t="e">
+      <c r="J31" s="46">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K31" s="47" t="e">
+        <v>-1</v>
+      </c>
+      <c r="K31" s="47">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L31" s="48">
         <f t="shared" ref="L31" ca="1" si="10">IF(NOW()&lt;B31, G31/_xlfn.DAYS(NOW(),B30), G31/_xlfn.DAYS(B31,B30))</f>
-        <v>0</v>
+        <v>-28</v>
       </c>
       <c r="M31" s="49">
         <f t="shared" ca="1" si="7"/>
@@ -2217,7 +2232,7 @@
       </c>
       <c r="O31" s="65">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-0.2857142857142857</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -2234,20 +2249,20 @@
         <v>0</v>
       </c>
       <c r="E32" s="42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="43" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="43" t="e">
-        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G32" s="44">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H32" s="45" t="e">
+      <c r="H32" s="45">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>-1</v>
       </c>
       <c r="I32" s="44">
         <f t="shared" ref="I32" si="11">D32-0</f>
@@ -2275,7 +2290,7 @@
       </c>
       <c r="O32" s="65">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2494,8 +2509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BDFBF0-BDE3-48CD-9C74-022AECEC1124}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2588,7 +2603,7 @@
       </c>
       <c r="C6" s="74"/>
       <c r="D6" s="73" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="E6" s="73" t="s">
         <v>53</v>
@@ -2784,7 +2799,7 @@
       </c>
       <c r="C18" s="74"/>
       <c r="D18" s="73" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="E18" s="73" t="s">
         <v>53</v>
@@ -2811,33 +2826,62 @@
       <c r="A20" s="73">
         <v>16</v>
       </c>
-      <c r="C20" s="74"/>
+      <c r="B20" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="74" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="73" t="s">
+        <v>32</v>
+      </c>
       <c r="G20" s="74"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="73">
         <v>17</v>
       </c>
+      <c r="B21" s="73" t="s">
+        <v>83</v>
+      </c>
       <c r="C21" s="74"/>
+      <c r="D21" s="73" t="s">
+        <v>73</v>
+      </c>
       <c r="G21" s="74"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="73">
         <v>18</v>
       </c>
+      <c r="B22" s="73" t="s">
+        <v>84</v>
+      </c>
       <c r="C22" s="74"/>
+      <c r="D22" s="73" t="s">
+        <v>73</v>
+      </c>
       <c r="G22" s="74"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="73">
         <v>19</v>
       </c>
+      <c r="B23" s="73" t="s">
+        <v>85</v>
+      </c>
       <c r="C23" s="74"/>
+      <c r="D23" s="73" t="s">
+        <v>19</v>
+      </c>
       <c r="G23" s="74"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="73">
         <v>20</v>
+      </c>
+      <c r="B24" s="73" t="s">
+        <v>86</v>
       </c>
       <c r="C24" s="74"/>
       <c r="G24" s="74"/>

</xml_diff>